<commit_message>
add my notes to opt-table
</commit_message>
<xml_diff>
--- a/synthetic_query_gen/notebooks/data/for_paper/opt_table.xlsx
+++ b/synthetic_query_gen/notebooks/data/for_paper/opt_table.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cherlihy3/Dropbox (GaTech)/ClarityNLPOptimized/synthetic_query_gen/notebooks/data/for_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charityhilton/repos/ClarityNLPOptimized/synthetic_query_gen/notebooks/data/for_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4B3D9747-2505-3347-AEDD-31AE4B92CA9A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16140" xr2:uid="{93543E86-FD46-5046-9F2C-AADC6E8D73DE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t xml:space="preserve">Optimization </t>
   </si>
@@ -75,9 +80,6 @@
     <t>Cache of commonly occurring query predicates</t>
   </si>
   <si>
-    <t>Allow the results of query 1 to be</t>
-  </si>
-  <si>
     <t>Pre-compute downselection of each query primitive. Then, reorder synthetic query so that sub-clauses containing primitives with greater downselection potential get executed first.</t>
   </si>
   <si>
@@ -88,12 +90,33 @@
   </si>
   <si>
     <t>Implement least recently used (LRU) caching</t>
+  </si>
+  <si>
+    <t>Run queries such that queries where all predicates contain only 'AND' are chained. Results from NLPQL 1, must complete before NLPQL 2 is ran, and the document set of query 2 is limited to only matches found in query 1.</t>
+  </si>
+  <si>
+    <t>Note: There has been effort on the main ClarityNLP project to implement this with MongoDB, but we did not evaluate it for this project.</t>
+  </si>
+  <si>
+    <t>Cache commonly used objects in queries, such as documents and Python objects preloaded with models and regular expressions. Cache results of NLPQL queries given a hash of query parameters. This was implemented using the cachetools library with a max size of 5000.</t>
+  </si>
+  <si>
+    <t>We evaluated existing indices. At this time all commonly used keys are indexed. However, a future application might be to use a deep learning model to determine where additional indexes would be helpful. In addition, our evaluation is primarily focused on computation and writes, while indexes generally help on read applications.</t>
+  </si>
+  <si>
+    <t>Two common tasks in the ClarityNLP pipeline are segmentation of notes by section and sentence. The former uses a custom ClarityNLP library and the latter uses spacy. Both are computationally intense. For every document in the evaluation Solr index, we ran and stored the sections and sentences as arrays in Solr, which can be retrieved rather than re-computed.</t>
+  </si>
+  <si>
+    <t>Redis is a commonly used in-memory key-value data store. This activity primarily compares Redis against a LRU cache as discussed above. Redis is slightly less amenable to data in ClarityNLP, as most cached items require some serialization.</t>
+  </si>
+  <si>
+    <t>Luigi works are somewhat constrained by CPUs in a system. However, in theory ClarityNLP + Luigi could be evaluated by comparing the same NLPQL query across different configurations of ClarityNLP batch sizes and Luigi workers. We ran additional configurations to capture performance, but did not build a model for this task.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -103,19 +126,13 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -127,174 +144,174 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -323,9 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -350,9 +364,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -373,6 +384,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,11 +704,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60317595-5DDB-8143-B2D5-981CBEADBE87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,135 +723,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="10">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="6">
         <v>0</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17">
-        <v>1</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="C7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="C8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -846,37 +871,41 @@
       <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="D10" s="6">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17">
-        <v>1</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="C11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
         <v>1</v>
       </c>
     </row>

</xml_diff>